<commit_message>
hardware bom and gerb updates
</commit_message>
<xml_diff>
--- a/hardware/Opo_v4/Project Outputs for opo4/BOM/Bill of Materials-opo4.xlsx
+++ b/hardware/Opo_v4/Project Outputs for opo4/BOM/Bill of Materials-opo4.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="218">
   <si>
     <t>Designator</t>
   </si>
@@ -72,18 +72,6 @@
     <t>712-1536-1-ND</t>
   </si>
   <si>
-    <t>BC1</t>
-  </si>
-  <si>
-    <t>2-pin JST-PH 2mm Battery Connector</t>
-  </si>
-  <si>
-    <t>Sparkfun</t>
-  </si>
-  <si>
-    <t>PRT-08612</t>
-  </si>
-  <si>
     <t>C1, C3</t>
   </si>
   <si>
@@ -126,6 +114,9 @@
     <t>C5</t>
   </si>
   <si>
+    <t>4.7 uF</t>
+  </si>
+  <si>
     <t>4.7 uF 10% 0402 6.3V X5R ceramic cap</t>
   </si>
   <si>
@@ -147,6 +138,9 @@
     <t>C7</t>
   </si>
   <si>
+    <t>33 nF</t>
+  </si>
+  <si>
     <t>33nF 10% 0402 16V X7R ceramic cap</t>
   </si>
   <si>
@@ -156,6 +150,9 @@
     <t>C8</t>
   </si>
   <si>
+    <t>2.2 nF</t>
+  </si>
+  <si>
     <t>2.2nF 10% 50V X7R ceramic cap</t>
   </si>
   <si>
@@ -201,9 +198,6 @@
     <t>C34</t>
   </si>
   <si>
-    <t>4.7 uF</t>
-  </si>
-  <si>
     <t>Tantalum capacitor, 4.7 uF, 0603 package</t>
   </si>
   <si>
@@ -234,6 +228,9 @@
     <t>C56, C57, C58</t>
   </si>
   <si>
+    <t>39 pF</t>
+  </si>
+  <si>
     <t>Ceramic capacitor, 0402, 39 pF, 5%, C0G, NP0, RF suitable</t>
   </si>
   <si>
@@ -363,7 +360,7 @@
     <t>541-2.20LLCT-ND</t>
   </si>
   <si>
-    <t>R4, R5, R6, R10, R11, R13</t>
+    <t>R5, R6, R10, R11, R13</t>
   </si>
   <si>
     <t>100K</t>
@@ -510,10 +507,10 @@
     <t>U2</t>
   </si>
   <si>
-    <t>Rf Switch</t>
-  </si>
-  <si>
-    <t>1465-1373-1-ND</t>
+    <t>GaAs Integrated Circuit for L, S-Band SPDT Switch</t>
+  </si>
+  <si>
+    <t>UPG2214TB-E4-ACT-ND</t>
   </si>
   <si>
     <t>U3</t>
@@ -627,13 +624,10 @@
     <t>U16</t>
   </si>
   <si>
-    <t>IC INVERTER DUAL SCHMTRIG ULLGA6</t>
-  </si>
-  <si>
-    <t>Mouser</t>
-  </si>
-  <si>
-    <t>863-NLX2G14BMX1TCG</t>
+    <t>1 uA supply current, 50 mA output current, Dual inverter</t>
+  </si>
+  <si>
+    <t>NC7WZ14L6XFSCT-ND</t>
   </si>
   <si>
     <t>UT1</t>
@@ -1028,7 +1022,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F61"/>
+  <dimension ref="A1:F60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1122,16 +1116,16 @@
         <v>17</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D5" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>20</v>
@@ -1148,30 +1142,30 @@
         <v>23</v>
       </c>
       <c r="D6" s="3">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D7" s="3">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>29</v>
@@ -1188,10 +1182,10 @@
         <v>32</v>
       </c>
       <c r="D8" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>33</v>
@@ -1202,50 +1196,50 @@
         <v>34</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D9" s="3">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D10" s="3">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D11" s="3">
         <v>1</v>
@@ -1254,18 +1248,18 @@
         <v>9</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>7</v>
+        <v>47</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D12" s="3">
         <v>1</v>
@@ -1274,258 +1268,258 @@
         <v>9</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="D13" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D14" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D15" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D16" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D17" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D18" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D19" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D20" s="3">
         <v>1</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D21" s="3">
         <v>1</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D22" s="3">
         <v>1</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D23" s="3">
         <v>1</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>7</v>
+        <v>88</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="D24" s="3">
         <v>1</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="D25" s="3">
         <v>1</v>
@@ -1534,78 +1528,78 @@
         <v>9</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>93</v>
+        <v>7</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D26" s="3">
         <v>1</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D27" s="3">
         <v>1</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>7</v>
+        <v>102</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="D28" s="3">
         <v>1</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="D29" s="3">
         <v>1</v>
@@ -1614,18 +1608,18 @@
         <v>9</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="D30" s="3">
         <v>1</v>
@@ -1634,238 +1628,238 @@
         <v>9</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="D31" s="3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="D32" s="3">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="D33" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="D34" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D35" s="3">
         <v>2</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="D36" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="D37" s="3">
         <v>1</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="D38" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="D39" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="D40" s="3">
         <v>1</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>9</v>
+        <v>152</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="D41" s="3">
         <v>1</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>153</v>
+        <v>9</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>156</v>
+        <v>7</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="D42" s="3">
         <v>1</v>
@@ -1874,38 +1868,38 @@
         <v>9</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="D43" s="3">
         <v>1</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="D44" s="3">
         <v>1</v>
@@ -1914,18 +1908,18 @@
         <v>9</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="D45" s="3">
         <v>1</v>
@@ -1934,278 +1928,278 @@
         <v>9</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="D46" s="3">
         <v>1</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="D47" s="3">
         <v>1</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="D48" s="3">
         <v>1</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="D49" s="3">
         <v>1</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="D50" s="3">
         <v>1</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="D51" s="3">
         <v>1</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="D52" s="3">
         <v>1</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="D53" s="3">
         <v>1</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="D54" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="D55" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D56" s="3">
         <v>1</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="D57" s="3">
         <v>1</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>203</v>
+        <v>24</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>7</v>
+        <v>207</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="D58" s="3">
         <v>1</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="D59" s="3">
         <v>1</v>
@@ -2214,47 +2208,27 @@
         <v>9</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>213</v>
+        <v>7</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D60" s="3">
         <v>1</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>9</v>
+        <v>216</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C61" s="2" t="s">
         <v>217</v>
-      </c>
-      <c r="D61" s="3">
-        <v>1</v>
-      </c>
-      <c r="E61" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="F61" s="2" t="s">
-        <v>219</v>
       </c>
     </row>
   </sheetData>

</xml_diff>